<commit_message>
Co-authored-by: ach rusdie <achrusdi@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/public/xlsx/test.xlsx
+++ b/public/xlsx/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\smati\public\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38638F50-2105-41E3-B78A-8EE0FA87272A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E1C288-C272-4BAC-94EF-A5B0C382BF6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D62F6702-42EB-4131-954E-A03F08797514}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7995" xr2:uid="{D62F6702-42EB-4131-954E-A03F08797514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>no</t>
   </si>
@@ -45,22 +45,19 @@
     <t>nama_merk</t>
   </si>
   <si>
+    <t>Headset Logitec</t>
+  </si>
+  <si>
+    <t>HD/0010/2019</t>
+  </si>
+  <si>
+    <t>HD/0011/2019</t>
+  </si>
+  <si>
     <t>HD/0001/2019</t>
   </si>
   <si>
-    <t>Headset Logitec</t>
-  </si>
-  <si>
     <t>HD/0002/2019</t>
-  </si>
-  <si>
-    <t>HD/0010/2019</t>
-  </si>
-  <si>
-    <t>HD/0011/2019</t>
-  </si>
-  <si>
-    <t>HD/0012/2019</t>
   </si>
 </sst>
 </file>
@@ -418,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F960D5A3-6A69-4519-A353-C860B171CA4C}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,13 +447,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -464,13 +461,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -478,13 +475,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,52 +489,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>